<commit_message>
Avance estable: login, registro, mantenimiento con mensajes y animaciones
</commit_message>
<xml_diff>
--- a/static/hojas_vida/CALIDAD_1CFYFC1.xlsx
+++ b/static/hojas_vida/CALIDAD_1CFYFC1.xlsx
@@ -2511,9 +2511,17 @@
       </c>
     </row>
     <row r="34" ht="164.25" customHeight="1" s="44">
-      <c r="A34" s="18" t="n"/>
+      <c r="A34" s="18" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
       <c r="B34" s="131" t="n"/>
-      <c r="C34" s="18" t="n"/>
+      <c r="C34" s="18" t="inlineStr">
+        <is>
+          <t>uuuuuuu</t>
+        </is>
+      </c>
       <c r="D34" s="130" t="n"/>
       <c r="E34" s="130" t="n"/>
       <c r="F34" s="130" t="n"/>
@@ -2523,7 +2531,11 @@
       <c r="J34" s="130" t="n"/>
       <c r="K34" s="130" t="n"/>
       <c r="L34" s="131" t="n"/>
-      <c r="M34" s="18" t="n"/>
+      <c r="M34" s="18" t="inlineStr">
+        <is>
+          <t>SV Romero Romero Miguel Ángel</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="168" customHeight="1" s="44">
       <c r="A35" s="18" t="n"/>

</xml_diff>

<commit_message>
✅ Proyecto finalizado: todos los módulos activos y probados
</commit_message>
<xml_diff>
--- a/static/hojas_vida/CALIDAD_1CFYFC1.xlsx
+++ b/static/hojas_vida/CALIDAD_1CFYFC1.xlsx
@@ -2511,9 +2511,17 @@
       </c>
     </row>
     <row r="34" ht="164.25" customHeight="1" s="44">
-      <c r="A34" s="18" t="n"/>
+      <c r="A34" s="18" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
       <c r="B34" s="131" t="n"/>
-      <c r="C34" s="18" t="n"/>
+      <c r="C34" s="18" t="inlineStr">
+        <is>
+          <t>uuuuuuu</t>
+        </is>
+      </c>
       <c r="D34" s="130" t="n"/>
       <c r="E34" s="130" t="n"/>
       <c r="F34" s="130" t="n"/>
@@ -2523,12 +2531,24 @@
       <c r="J34" s="130" t="n"/>
       <c r="K34" s="130" t="n"/>
       <c r="L34" s="131" t="n"/>
-      <c r="M34" s="18" t="n"/>
+      <c r="M34" s="18" t="inlineStr">
+        <is>
+          <t>SV Romero Romero Miguel Ángel</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="168" customHeight="1" s="44">
-      <c r="A35" s="18" t="n"/>
+      <c r="A35" s="18" t="inlineStr">
+        <is>
+          <t>2025-05-26</t>
+        </is>
+      </c>
       <c r="B35" s="131" t="n"/>
-      <c r="C35" s="18" t="n"/>
+      <c r="C35" s="18" t="inlineStr">
+        <is>
+          <t>clon 2222222</t>
+        </is>
+      </c>
       <c r="D35" s="130" t="n"/>
       <c r="E35" s="130" t="n"/>
       <c r="F35" s="130" t="n"/>
@@ -2538,7 +2558,11 @@
       <c r="J35" s="130" t="n"/>
       <c r="K35" s="130" t="n"/>
       <c r="L35" s="131" t="n"/>
-      <c r="M35" s="18" t="n"/>
+      <c r="M35" s="18" t="inlineStr">
+        <is>
+          <t>SV Romero Romero Miguel Ángel</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="166.5" customHeight="1" s="44">
       <c r="A36" s="18" t="n"/>

</xml_diff>

<commit_message>
Diseño de .bat acceso directo
</commit_message>
<xml_diff>
--- a/static/hojas_vida/CALIDAD_1CFYFC1.xlsx
+++ b/static/hojas_vida/CALIDAD_1CFYFC1.xlsx
@@ -2565,9 +2565,17 @@
       </c>
     </row>
     <row r="36" ht="166.5" customHeight="1" s="44">
-      <c r="A36" s="18" t="n"/>
+      <c r="A36" s="18" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
       <c r="B36" s="131" t="n"/>
-      <c r="C36" s="18" t="n"/>
+      <c r="C36" s="18" t="inlineStr">
+        <is>
+          <t>22222</t>
+        </is>
+      </c>
       <c r="D36" s="130" t="n"/>
       <c r="E36" s="130" t="n"/>
       <c r="F36" s="130" t="n"/>
@@ -2577,12 +2585,24 @@
       <c r="J36" s="130" t="n"/>
       <c r="K36" s="130" t="n"/>
       <c r="L36" s="131" t="n"/>
-      <c r="M36" s="18" t="n"/>
+      <c r="M36" s="18" t="inlineStr">
+        <is>
+          <t>SV Romero Romero Miguel Ángel</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="168.75" customHeight="1" s="44">
-      <c r="A37" s="18" t="n"/>
+      <c r="A37" s="18" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
       <c r="B37" s="131" t="n"/>
-      <c r="C37" s="18" t="n"/>
+      <c r="C37" s="18" t="inlineStr">
+        <is>
+          <t>jjjjj</t>
+        </is>
+      </c>
       <c r="D37" s="130" t="n"/>
       <c r="E37" s="130" t="n"/>
       <c r="F37" s="130" t="n"/>
@@ -2592,12 +2612,24 @@
       <c r="J37" s="130" t="n"/>
       <c r="K37" s="130" t="n"/>
       <c r="L37" s="131" t="n"/>
-      <c r="M37" s="18" t="n"/>
+      <c r="M37" s="18" t="inlineStr">
+        <is>
+          <t>SV Romero Romero Miguel Ángel</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="169.5" customHeight="1" s="44">
-      <c r="A38" s="18" t="n"/>
+      <c r="A38" s="18" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
       <c r="B38" s="131" t="n"/>
-      <c r="C38" s="18" t="n"/>
+      <c r="C38" s="18" t="inlineStr">
+        <is>
+          <t>cambio de ram</t>
+        </is>
+      </c>
       <c r="D38" s="130" t="n"/>
       <c r="E38" s="130" t="n"/>
       <c r="F38" s="130" t="n"/>
@@ -2607,7 +2639,11 @@
       <c r="J38" s="130" t="n"/>
       <c r="K38" s="130" t="n"/>
       <c r="L38" s="131" t="n"/>
-      <c r="M38" s="18" t="n"/>
+      <c r="M38" s="18" t="inlineStr">
+        <is>
+          <t>SV Romero Romero Miguel Ángel</t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="130.5" customHeight="1" s="44">
       <c r="A39" s="18" t="n"/>

</xml_diff>